<commit_message>
Additional Features, more Changes and more Bug Fixes
</commit_message>
<xml_diff>
--- a/data/CrownRoot.xlsx
+++ b/data/CrownRoot.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="315" windowWidth="24840" windowHeight="7950"/>
+    <workbookView xWindow="615" yWindow="315" windowWidth="24240" windowHeight="7950" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="34" r:id="rId1"/>
     <sheet name="CRLogin" sheetId="39" r:id="rId2"/>
     <sheet name="Navigate" sheetId="49" r:id="rId3"/>
     <sheet name="Process" sheetId="51" r:id="rId4"/>
-    <sheet name="ToDo" sheetId="32" r:id="rId5"/>
-    <sheet name="Codes" sheetId="52" r:id="rId6"/>
+    <sheet name="Search" sheetId="53" r:id="rId5"/>
+    <sheet name="ToDo" sheetId="32" r:id="rId6"/>
+    <sheet name="Codes" sheetId="52" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Action">Codes!$A$2:$A$102</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="151">
   <si>
     <t>Action</t>
   </si>
@@ -445,6 +446,39 @@
   </si>
   <si>
     <t>URL=https://demo-cf.donorfirst.org/;UserName=Jackie;User=Jackie_K;password=Demo2014;browser=Chrome</t>
+  </si>
+  <si>
+    <t>Search#</t>
+  </si>
+  <si>
+    <t>search_term</t>
+  </si>
+  <si>
+    <t>value=norman</t>
+  </si>
+  <si>
+    <t>Search for organizations with name containing Norman</t>
+  </si>
+  <si>
+    <t>Click the Search</t>
+  </si>
+  <si>
+    <t>InputSpecs=File!CrownRoot.xlsx!Search</t>
+  </si>
+  <si>
+    <t>Search for foundations</t>
+  </si>
+  <si>
+    <t>Firehouse</t>
+  </si>
+  <si>
+    <t>waitTime=3</t>
+  </si>
+  <si>
+    <t>Click the Norman Firehouse link</t>
+  </si>
+  <si>
+    <t>Wait a bit</t>
   </si>
 </sst>
 </file>
@@ -529,7 +563,217 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="108">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1420,11 +1664,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1509,7 +1753,7 @@
         <v>83</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I17" si="0">"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <f t="shared" ref="I3:I18" si="0">"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
         <v>list.add(new String[] {"CrPOC#",  "refreshSettings",  "",  "",  "",  "no",  "",  "Refresh The Settings"});</v>
       </c>
     </row>
@@ -1555,19 +1799,22 @@
       <c r="A6" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
+        <v>145</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!Navigate",  "Explore (navigation only) {UserName}'s perspective of the application"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!Search",  "Search for foundations"});</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1579,14 +1826,14 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!Process",  "Explore (and process) {UserName}'s perspective of the application"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!Navigate",  "Explore (navigation only) {UserName}'s perspective of the application"});</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1594,18 +1841,18 @@
         <v>120</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "generateReport",  "",  "",  "",  "",  "Description=Crown Test Session Results - FireFox",  "Generate the report for this session - Chrome browser"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!Process",  "Explore (and process) {UserName}'s perspective of the application"});</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1613,16 +1860,18 @@
         <v>120</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="I9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "quit",  "",  "",  "",  "",  "",  "Close and quit the driver if it still exists"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "generateReport",  "",  "",  "",  "",  "Description=Crown Test Session Results - FireFox",  "Generate the report for this session - Chrome browser"});</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1630,56 +1879,54 @@
         <v>120</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>126</v>
-      </c>
+      <c r="G10" s="4"/>
       <c r="H10" s="1" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "runCommand",  "",  "",  "",  "",  "FileName=%script%CopyReplace.Bat;Param1={$resourcesdir}firefox.properties;param2={$resourcesdir}ddt.properties;WaitTime=1",  "Replace properties file with one running on FireFox"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "quit",  "",  "",  "",  "",  "",  "Close and quit the driver if it still exists"});</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
+      <c r="B11" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "setVars",  "",  "",  "",  "",  "Browser=CHROME",  "Chenge Browser"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "runCommand",  "",  "",  "",  "",  "FileName=%script%CopyReplace.Bat;Param1={$resourcesdir}firefox.properties;param2={$resourcesdir}ddt.properties;WaitTime=1",  "Replace properties file with one running on FireFox"});</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!CRLogin;ptp=QTOF",  "Login with credentials of User={user}, Password={password}"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "setVars",  "",  "",  "",  "",  "Browser=CHROME",  "Chenge Browser"});</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1691,14 +1938,14 @@
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>22</v>
+        <v>119</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!Navigate",  "Explore (navigation only) {UserName}'s perspective of the application"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!CRLogin;ptp=QTOF",  "Login with credentials of User={user}, Password={password}"});</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1710,55 +1957,55 @@
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!Process",  "Explore (and process) {UserName}'s perspective of the application"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!Navigate",  "Explore (navigation only) {UserName}'s perspective of the application"});</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!%data%process/Crown/Dashboard.xlsx!Search Grantee",  "Search Grantee and Make a Grant for it"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!CrownRoot.xlsx!Process",  "Explore (and process) {UserName}'s perspective of the application"});</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>81</v>
+        <v>127</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "generateReport",  "",  "",  "",  "",  "Description=Crown Test Session Results - CHROME",  "Generate the report for this session - FireFox Browser"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "newTest",  "",  "",  "",  "",  "InputSpecs=File!%data%process/Crown/Dashboard.xlsx!Search Grantee",  "Search Grantee and Make a Grant for it"});</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1766,31 +2013,50 @@
         <v>120</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="H17" s="1" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
+        <v>list.add(new String[] {"CrPOC#",  "generateReport",  "",  "",  "",  "",  "Description=Crown Test Session Results - CHROME",  "Generate the report for this session - FireFox Browser"});</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="H18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>list.add(new String[] {"CrPOC#",  "quit",  "",  "",  "",  "",  "",  "Close and quit the driver if it still exists"});</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H16 H10:H14 H5:H8 H1:H3">
-    <cfRule type="cellIs" dxfId="79" priority="66" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="67" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="68" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16 H10:H14 H5:H8 H1:H3">
-    <cfRule type="cellIs" dxfId="76" priority="65" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="H17 H11:H15 H5:H9 H1:H3">
+    <cfRule type="cellIs" dxfId="3" priority="66" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="67" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="68" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17 H11:H15 H5:H9 H1:H3">
+    <cfRule type="cellIs" dxfId="0" priority="65" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1806,7 +2072,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G15" r:id="rId1" display="FileName=@data@process\Crown\Dashboard.xlsx;WorksheetName=Make A Grant"/>
+    <hyperlink ref="G16" r:id="rId1" display="FileName=@data@process\Crown\Dashboard.xlsx;WorksheetName=Make A Grant"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2035,114 +2301,114 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="75" priority="26" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="27" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="28" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="72" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="26" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="27" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="28" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="104" priority="25" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H6">
-    <cfRule type="cellIs" dxfId="71" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="24" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H6">
-    <cfRule type="cellIs" dxfId="68" priority="21" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="67" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="64" priority="17" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="63" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="16" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="60" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="59" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="56" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="55" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="52" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="51" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="48" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="99" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="96" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="95" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="92" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="91" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="88" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="87" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="84" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="83" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="80" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2313,98 +2579,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="47" priority="58" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="59" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="60" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="44" priority="57" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="43" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="40" priority="17" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="39" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="16" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="36" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="35" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="32" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="31" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="28" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="27" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="58" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="59" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="60" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="76" priority="57" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="75" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="72" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="71" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="68" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="67" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="64" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="63" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="60" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="59" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="56" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2576,98 +2842,98 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="23" priority="22" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="23" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="20" priority="21" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="19" priority="18" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="19" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="20" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="15" priority="14" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="12" priority="13" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="11" priority="10" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="8" priority="9" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="24" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="52" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="51" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="48" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="47" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="44" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="43" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="40" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="39" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="36" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="35" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2688,6 +2954,316 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9" style="7" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="7"/>
+    <col min="7" max="7" width="42.85546875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="34.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="52.7109375" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="7" t="str">
+        <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Search#",  "sendKeys",  "Name",  "search_term",  "",  "",  "value=norman",  "Search for organizations with name containing Norman"});</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="7" t="str">
+        <f t="shared" ref="I3:I5" si="0">"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
+        <v>list.add(new String[] {"Search#",  "click",  "id",  "edit-submit",  "",  "",  "",  "Click the Search"});</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>list.add(new String[] {"Search#",  "wait",  "",  "",  "",  "",  "waitTime=3",  "Wait a bit"});</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>list.add(new String[] {"Search#",  "click",  "PartialLinkText",  "Firehouse",  "",  "",  "",  "Click the Norman Firehouse link"});</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="31" priority="22" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="23" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="24" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="28" priority="21" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="27" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="19" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="20" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="24" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="23" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="20" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="19" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="16" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+      <formula1>Query</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+      <formula1>Locator</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+      <formula1>Action</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="FileName=@data@navigate\Crown\Dashboard.xlsx;WorksheetName=Navigate"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2824,7 +3400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H28"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Tab Delimited text file as input source
</commit_message>
<xml_diff>
--- a/data/CrownRoot.xlsx
+++ b/data/CrownRoot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="420" windowWidth="24240" windowHeight="7950"/>
+    <workbookView xWindow="780" yWindow="420" windowWidth="24240" windowHeight="7950" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="34" r:id="rId1"/>
@@ -12,20 +12,19 @@
     <sheet name="Navigate" sheetId="49" r:id="rId3"/>
     <sheet name="Process" sheetId="51" r:id="rId4"/>
     <sheet name="Search" sheetId="53" r:id="rId5"/>
-    <sheet name="ToDo" sheetId="32" r:id="rId6"/>
-    <sheet name="Codes" sheetId="52" r:id="rId7"/>
+    <sheet name="Codes" sheetId="52" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="Action">Codes!$A$2:$A$102</definedName>
+    <definedName name="Action">Codes!$A$2:$A$107</definedName>
     <definedName name="Locator">Codes!$C$2:$C6</definedName>
-    <definedName name="Query">Codes!$E$2:$E$22</definedName>
+    <definedName name="Query">Codes!$E$2:$E$25</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="122">
   <si>
     <t>Action</t>
   </si>
@@ -120,9 +119,6 @@
     <t>Close and quit the driver if it still exists</t>
   </si>
   <si>
-    <t>CrPOC03</t>
-  </si>
-  <si>
     <t>edit-name</t>
   </si>
   <si>
@@ -138,15 +134,9 @@
     <t>Verify the navigation page is loaded</t>
   </si>
   <si>
-    <t>CRLogin02</t>
-  </si>
-  <si>
     <t>Process tabs and subtabs of the Dashboard page</t>
   </si>
   <si>
-    <t>CRLogin07</t>
-  </si>
-  <si>
     <t>ClassName</t>
   </si>
   <si>
@@ -219,9 +209,6 @@
     <t>IsDisplayed</t>
   </si>
   <si>
-    <t>findPage</t>
-  </si>
-  <si>
     <t>Xpath</t>
   </si>
   <si>
@@ -246,9 +233,6 @@
     <t>setPageSize</t>
   </si>
   <si>
-    <t>switchToFrame</t>
-  </si>
-  <si>
     <t>takeScreenShot</t>
   </si>
   <si>
@@ -288,97 +272,12 @@
     <t>Login with credentials of User={user}, Password={password}</t>
   </si>
   <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>Worksheet</t>
-  </si>
-  <si>
-    <t>Step</t>
-  </si>
-  <si>
-    <t>Reuse - Factoring</t>
-  </si>
-  <si>
-    <t>CRLogin</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Reuse - Static Variable</t>
-  </si>
-  <si>
-    <t>Root</t>
-  </si>
-  <si>
-    <t>MakeGrantDetail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MakeAGrant27,MakeAGrant28
-</t>
-  </si>
-  <si>
-    <t>How long to wait</t>
-  </si>
-  <si>
-    <t>Make A Contribution</t>
-  </si>
-  <si>
-    <t>Date-Dependent</t>
-  </si>
-  <si>
-    <t>Post Test Policy</t>
-  </si>
-  <si>
-    <t>CRLogin, Navigation</t>
-  </si>
-  <si>
-    <t>Screen Shots</t>
-  </si>
-  <si>
-    <t>Insert in CR Login as last step</t>
-  </si>
-  <si>
-    <t>CRLogin08</t>
-  </si>
-  <si>
-    <t>Go over logic / preoperties</t>
-  </si>
-  <si>
-    <t>Reporting Control</t>
-  </si>
-  <si>
-    <t>PhantomDriver</t>
-  </si>
-  <si>
-    <t>Reporting with Listener</t>
-  </si>
-  <si>
-    <t>Reporting hierarchy</t>
-  </si>
-  <si>
-    <t>Resolve Quit issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Explore verifying with Assertions </t>
-  </si>
-  <si>
-    <t>HtmlTestItemProvider</t>
-  </si>
-  <si>
-    <t>Independence of column order in xls / xlsx</t>
-  </si>
-  <si>
     <t>Description=Crown Test Session Results - FireFox</t>
   </si>
   <si>
     <t>Value=Dashboard;CompareMode=Equals;WaitTime=10;ptp=QSOF</t>
   </si>
   <si>
-    <t>Implement Between, isLowerCase, isUpperCase, between,in(separated;options;at large;</t>
-  </si>
-  <si>
     <t>InputSpecs=File!CrownRoot.xlsx!Navigate</t>
   </si>
   <si>
@@ -400,12 +299,6 @@
     <t>Dashboard#</t>
   </si>
   <si>
-    <t>Done - has problems</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>FileName=%script%CopyReplace.Bat;Param1={$resourcesdir}firefox.properties;param2={$resourcesdir}ddt.properties;WaitTime=1</t>
   </si>
   <si>
@@ -479,13 +372,31 @@
   </si>
   <si>
     <t>Wait a bit</t>
+  </si>
+  <si>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>runExternalMethod</t>
+  </si>
+  <si>
+    <t>runJS</t>
+  </si>
+  <si>
+    <t>switchTo</t>
+  </si>
+  <si>
+    <t>verify</t>
+  </si>
+  <si>
+    <t>verifyElementSize</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,12 +411,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -549,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -558,7 +463,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1636,9 +1540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1683,22 +1587,22 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I2" s="2" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
@@ -1707,20 +1611,20 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I18" si="0">"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
@@ -1729,17 +1633,17 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1748,17 +1652,17 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1767,7 +1671,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>19</v>
@@ -1777,10 +1681,10 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1789,14 +1693,14 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>22</v>
@@ -1808,14 +1712,14 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>23</v>
@@ -1827,17 +1731,17 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1846,7 +1750,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -1863,17 +1767,17 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1882,17 +1786,17 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1901,17 +1805,17 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1920,14 +1824,14 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>22</v>
@@ -1939,14 +1843,14 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>23</v>
@@ -1958,7 +1862,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>19</v>
@@ -1968,10 +1872,10 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1980,17 +1884,17 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1999,7 +1903,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>10</v>
@@ -2097,7 +2001,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -2107,7 +2011,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>16</v>
@@ -2119,7 +2023,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -2131,7 +2035,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>20</v>
@@ -2143,7 +2047,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -2152,7 +2056,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2169,7 +2073,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -2178,7 +2082,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2195,16 +2099,16 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2219,7 +2123,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -2231,10 +2135,10 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -2243,26 +2147,26 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -2447,7 +2351,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -2457,7 +2361,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>21</v>
@@ -2710,7 +2614,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -2720,10 +2624,10 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I2" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
@@ -2973,24 +2877,24 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="I2" s="7" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
@@ -2999,22 +2903,22 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="I3" s="7" t="str">
         <f t="shared" ref="I3:I5" si="0">"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
@@ -3023,20 +2927,20 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="I4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -3045,22 +2949,22 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="I5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -3234,148 +3138,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="99.42578125" customWidth="1"/>
-    <col min="2" max="2" width="80.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="7" customFormat="1">
-      <c r="A4" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75">
-      <c r="A7" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75">
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:2" ht="15.75">
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:2" ht="15.75">
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:2" ht="15.75">
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:2" ht="15.75">
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:2" ht="15.75">
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:2" ht="15.75">
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:2" ht="15.75">
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="2:2" ht="15.75">
-      <c r="B17" s="8"/>
-    </row>
-    <row r="19" spans="2:2" ht="15.75">
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="2:2" ht="15.75">
-      <c r="B20" s="8"/>
-    </row>
-    <row r="22" spans="2:2" ht="15.75">
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="2:2" ht="15.75">
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="2:2" ht="15.75">
-      <c r="B24" s="8"/>
-    </row>
-    <row r="25" spans="2:2" ht="15.75">
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="2:2" ht="15.75">
-      <c r="B26" s="8"/>
-    </row>
-    <row r="27" spans="2:2" ht="15.75">
-      <c r="B27" s="8"/>
-    </row>
-    <row r="28" spans="2:2" ht="15.75">
-      <c r="B28" s="8"/>
-    </row>
-    <row r="29" spans="2:2" ht="15.75">
-      <c r="B29" s="8"/>
-    </row>
-    <row r="30" spans="2:2" ht="15.75">
-      <c r="B30" s="8"/>
-    </row>
-    <row r="32" spans="2:2" ht="15.75">
-      <c r="B32" s="8"/>
-    </row>
-    <row r="33" spans="2:2" ht="15.75">
-      <c r="B33" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3395,60 +3161,42 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>89</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>92</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>31</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
@@ -3458,131 +3206,99 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>39</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>96</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>98</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>104</v>
-      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>105</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>68</v>
+      <c r="A11" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="7" customFormat="1">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3597,77 +3313,97 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="3" customFormat="1">
-      <c r="A17" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="7" customFormat="1">
+      <c r="A17" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="7" customFormat="1">
+      <c r="A18" s="7" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="A19" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="3" customFormat="1">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>75</v>
+      <c r="A24" s="7" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" s="7" customFormat="1">
+      <c r="A27" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" s="7" customFormat="1">
+      <c r="A28" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>78</v>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33:B36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38:B41">
       <formula1>Action</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added JSON file as input source & Refactored some TestStringProvider methods.
</commit_message>
<xml_diff>
--- a/data/CrownRoot.xlsx
+++ b/data/CrownRoot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="420" windowWidth="24240" windowHeight="7950" activeTab="5"/>
+    <workbookView xWindow="780" yWindow="420" windowWidth="24180" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="34" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="122">
   <si>
     <t>Action</t>
   </si>
@@ -317,9 +317,6 @@
     <t>Browser=CHROME</t>
   </si>
   <si>
-    <t>Chenge Browser</t>
-  </si>
-  <si>
     <t>Description=Crown Test Session Results - CHROME</t>
   </si>
   <si>
@@ -390,6 +387,9 @@
   </si>
   <si>
     <t>verifyElementSize</t>
+  </si>
+  <si>
+    <t>Change Browser</t>
   </si>
 </sst>
 </file>
@@ -1540,9 +1540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1596,10 +1596,10 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>80</v>
@@ -1620,7 +1620,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>95</v>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>81</v>
@@ -1681,10 +1681,10 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1772,7 +1772,9 @@
       <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="G11" s="4" t="s">
         <v>91</v>
       </c>
@@ -1781,7 +1783,7 @@
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "runCommand",  "",  "",  "",  "",  "FileName=%script%CopyReplace.Bat;Param1={$resourcesdir}firefox.properties;param2={$resourcesdir}ddt.properties;WaitTime=1",  "Replace properties file with one running on FireFox"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "runCommand",  "",  "",  "",  "no",  "FileName=%script%CopyReplace.Bat;Param1={$resourcesdir}firefox.properties;param2={$resourcesdir}ddt.properties;WaitTime=1",  "Replace properties file with one running on FireFox"});</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1796,11 +1798,11 @@
         <v>96</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>list.add(new String[] {"CrPOC#",  "setVars",  "",  "",  "",  "",  "Browser=CHROME",  "Chenge Browser"});</v>
+        <v>list.add(new String[] {"CrPOC#",  "setVars",  "",  "",  "",  "",  "Browser=CHROME",  "Change Browser"});</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1891,7 +1893,7 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>76</v>
@@ -2011,7 +2013,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>16</v>
@@ -2035,7 +2037,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>20</v>
@@ -2877,7 +2879,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -2886,15 +2888,15 @@
         <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="I2" s="7" t="str">
         <f>"list.add(new String[] {" &amp; """" &amp; A2 &amp; """" &amp; ",  " &amp; """" &amp; B2 &amp; """" &amp; ",  " &amp; """" &amp; C2 &amp; """" &amp; ",  " &amp; """" &amp; D2 &amp;  """" &amp;  ",  " &amp; """" &amp; E2 &amp; """" &amp; ",  " &amp; """" &amp; F2 &amp; """" &amp; ",  " &amp; """" &amp; G2 &amp; """" &amp; ",  " &amp; """" &amp; H2 &amp; """" &amp; "});"</f>
@@ -2903,7 +2905,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2918,7 +2920,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I3" s="7" t="str">
         <f t="shared" ref="I3:I5" si="0">"list.add(new String[] {" &amp; """" &amp; A3 &amp; """" &amp; ",  " &amp; """" &amp; B3 &amp; """" &amp; ",  " &amp; """" &amp; C3 &amp; """" &amp; ",  " &amp; """" &amp; D3 &amp;  """" &amp;  ",  " &amp; """" &amp; E3 &amp; """" &amp; ",  " &amp; """" &amp; F3 &amp; """" &amp; ",  " &amp; """" &amp; G3 &amp; """" &amp; ",  " &amp; """" &amp; H3 &amp; """" &amp; "});"</f>
@@ -2927,7 +2929,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>73</v>
@@ -2937,10 +2939,10 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2949,7 +2951,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
@@ -2958,13 +2960,13 @@
         <v>57</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -3140,7 +3142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -3290,7 +3292,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E11" t="s">
         <v>63</v>
@@ -3323,12 +3325,12 @@
     </row>
     <row r="17" spans="1:1" s="7" customFormat="1">
       <c r="A17" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:1" s="7" customFormat="1">
       <c r="A18" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -3358,7 +3360,7 @@
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:1">
@@ -3373,12 +3375,12 @@
     </row>
     <row r="27" spans="1:1" s="7" customFormat="1">
       <c r="A27" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:1" s="7" customFormat="1">
       <c r="A28" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:1">

</xml_diff>